<commit_message>
Fixed issues with current DB and cleaned up code
</commit_message>
<xml_diff>
--- a/backend/Project Sample Data/file-errors.xlsx
+++ b/backend/Project Sample Data/file-errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo\OneDrive\Desktop\128\GWA-Verifier\backend\Project Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB14731-39AC-4B7D-A03A-BFBC1BBBB717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDC7977-252D-43F4-B785-D5396C1C23F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="86">
   <si>
     <t>CRSE NO.</t>
   </si>
@@ -291,6 +291,12 @@
   <si>
     <t>2018-79231</t>
   </si>
+  <si>
+    <t>CMSC 198</t>
+  </si>
+  <si>
+    <t>midyear 2021</t>
+  </si>
 </sst>
 </file>
 
@@ -481,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -503,13 +509,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,10 +736,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -808,7 +816,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D6:D54" si="0">B6*C6</f>
+        <f t="shared" ref="D6:D55" si="0">B6*C6</f>
         <v>6.75</v>
       </c>
       <c r="E6" s="2">
@@ -900,7 +908,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>12</v>
@@ -1621,28 +1629,31 @@
     </row>
     <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
       </c>
       <c r="C43" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" s="2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="E43" s="2">
-        <f>SUM(D5:D43)</f>
-        <v>165</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="6"/>
-      <c r="I43" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="F43" s="20">
+        <v>3</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>10</v>
@@ -1651,191 +1662,191 @@
         <v>1</v>
       </c>
       <c r="D44" s="2">
-        <f>0</f>
         <v>0</v>
       </c>
       <c r="E44" s="2">
         <f>SUM(D5:D44)</f>
-        <v>165</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
+        <v>168</v>
+      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" s="6"/>
+      <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1.75</v>
+        <v>47</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C45" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="0"/>
-        <v>5.25</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="E45" s="2">
         <f>SUM(D5:D45)</f>
-        <v>170.25</v>
+        <v>168</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="C46" s="2">
         <v>3</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5.25</v>
       </c>
       <c r="E46" s="2">
         <f>SUM(D5:D46)</f>
-        <v>176.25</v>
+        <v>173.25</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
         <v>6</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="C47" s="2">
-        <v>3</v>
-      </c>
-      <c r="D47" s="2">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
       </c>
       <c r="E47" s="2">
         <f>SUM(D5:D47)</f>
-        <v>180.75</v>
+        <v>179.25</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="B48" s="2">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C48" s="2">
         <v>3</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>4.5</v>
       </c>
       <c r="E48" s="2">
         <f>SUM(D5:D48)</f>
-        <v>186</v>
-      </c>
+        <v>183.75</v>
+      </c>
+      <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B49" s="2">
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="C49" s="2">
         <v>3</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="E49" s="2">
         <f>SUM(D5:D49)</f>
-        <v>190.5</v>
-      </c>
-      <c r="F49" s="9">
-        <v>16</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I49" s="1">
-        <v>16</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="B50" s="2">
-        <v>1.25</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>70</v>
+        <v>1.5</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3</v>
       </c>
       <c r="D50" s="2">
-        <v>3.75</v>
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
       <c r="E50" s="2">
-        <v>194.25</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
+        <f>SUM(D5:D50)</f>
+        <v>193.5</v>
+      </c>
+      <c r="F50" s="9">
+        <v>17</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I50" s="1">
+        <v>16</v>
+      </c>
     </row>
     <row r="51" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B51" s="2">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2">
-        <v>3</v>
+        <v>1.25</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="E51" s="2">
-        <f>SUM(D5:D51)</f>
-        <v>197.25</v>
+        <v>194.25</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B52" s="2">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="C52" s="2">
         <v>3</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="E52" s="2">
         <f>SUM(D5:D52)</f>
-        <v>202.5</v>
+        <v>200.25</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="2">
         <v>1.75</v>
@@ -1849,91 +1860,112 @@
       </c>
       <c r="E53" s="2">
         <f>SUM(D5:D53)</f>
-        <v>207.75</v>
-      </c>
+        <v>205.5</v>
+      </c>
+      <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="E54" s="2">
+        <f>SUM(D5:D54)</f>
+        <v>210.75</v>
+      </c>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="14">
-        <v>1.75</v>
-      </c>
-      <c r="C54" s="13">
-        <v>3</v>
-      </c>
-      <c r="D54" s="13">
+      <c r="B55" s="14">
+        <v>1.75</v>
+      </c>
+      <c r="C55" s="13">
+        <v>3</v>
+      </c>
+      <c r="D55" s="13">
         <f t="shared" si="0"/>
         <v>5.25</v>
       </c>
-      <c r="E54" s="13">
-        <f>SUM(D5:D54)</f>
-        <v>213</v>
-      </c>
-      <c r="F54" s="9">
+      <c r="E55" s="13">
+        <f>SUM(D5:D55)</f>
+        <v>216</v>
+      </c>
+      <c r="F55" s="9">
         <v>14</v>
       </c>
-      <c r="G54" s="10" t="s">
+      <c r="G55" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I55" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="15">
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="15">
         <v>14</v>
       </c>
-      <c r="G55" s="16" t="s">
+      <c r="G56" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B56" s="1">
-        <f>SUM(C5:C54)</f>
-        <v>125</v>
-      </c>
-      <c r="E56" s="1">
-        <f>E54</f>
-        <v>213</v>
-      </c>
-    </row>
     <row r="57" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="1">
+        <f>SUM(C5:C55)</f>
+        <v>128</v>
+      </c>
+      <c r="E57" s="1">
+        <f>E55</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="1">
-        <f>E56/(SUM(I4:I54))</f>
-        <v>1.6771653543307086</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="B58" s="1">
+        <f>E57/(SUM(I4:I55))</f>
+        <v>1.7007874015748032</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1962,7 +1994,7 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7770,7 +7802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3EA3B3-238C-408A-9C88-AD19546D82D3}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -7791,7 +7823,7 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>